<commit_message>
Added some test stuff
.
</commit_message>
<xml_diff>
--- a/TimeSheetApp/Test Case List.xlsx
+++ b/TimeSheetApp/Test Case List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
   <si>
     <t>Test case name</t>
   </si>
@@ -127,13 +127,106 @@
   </si>
   <si>
     <t>The User has traveled to the login URL.</t>
+  </si>
+  <si>
+    <t>Conducted by Elite</t>
+  </si>
+  <si>
+    <t>Participating Actors</t>
+  </si>
+  <si>
+    <t>Flow of Events</t>
+  </si>
+  <si>
+    <t>2. The Elite logs into Timesheet.</t>
+  </si>
+  <si>
+    <t>Entry Condition</t>
+  </si>
+  <si>
+    <t>Exit Condition</t>
+  </si>
+  <si>
+    <t>Elite adds the profile to the system and Grunt/+ is given username/password.</t>
+  </si>
+  <si>
+    <t>Quality Requirements</t>
+  </si>
+  <si>
+    <t>AddUser_CommonCase</t>
+  </si>
+  <si>
+    <t>The Elite is given the Grunt's information</t>
+  </si>
+  <si>
+    <t>1. The Elite logs into Timesheet.</t>
+  </si>
+  <si>
+    <t>2. The Elite clicks the "Add New Member" button.</t>
+  </si>
+  <si>
+    <t>3. The Elite fills out the profile information for the new Grunt/+.</t>
+  </si>
+  <si>
+    <t>4. The Elite clicks the "Save New Member" button.</t>
+  </si>
+  <si>
+    <t>5. The Grunt/+ is notified that their profile has been created, and they are supplied with a username/password to log into the system.</t>
+  </si>
+  <si>
+    <t>2. The Prophet or CFO logs into Timesheet.</t>
+  </si>
+  <si>
+    <t>3. The Prophet or CFO clicks on the Grunt's name and clicks the Edit button.</t>
+  </si>
+  <si>
+    <t>4. The Prophet or CFO is presented with an Edit Profile form where they make the changes.</t>
+  </si>
+  <si>
+    <t>5. The Prophet or CFO clicks the "Save Changes" button.</t>
+  </si>
+  <si>
+    <t>6. The Grunt is sent a notification that changes were made to his or her profile.</t>
+  </si>
+  <si>
+    <t>Changes are made to the User's profile</t>
+  </si>
+  <si>
+    <t>ModifyUser_CommonCase</t>
+  </si>
+  <si>
+    <t>Conducted by Prophet, CFO</t>
+  </si>
+  <si>
+    <t>Grunt's personal information changes</t>
+  </si>
+  <si>
+    <t>1. The Prophet or CFO is notified of change of Grunts's information</t>
+  </si>
+  <si>
+    <t>Elite</t>
+  </si>
+  <si>
+    <t>1. The Elite is notified of the Grunt/+'s departure from the company.</t>
+  </si>
+  <si>
+    <t>3. The Elite clicks on the Grunt/+'s name and clicks the "Delete Member" button.</t>
+  </si>
+  <si>
+    <t>Grunt/+ leaves the company</t>
+  </si>
+  <si>
+    <t>Elite removes Grunt/+'s profile from the system</t>
+  </si>
+  <si>
+    <t>RemoveUser_CommonCase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,6 +253,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -191,7 +292,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -209,13 +310,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -224,6 +338,11 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -232,6 +351,11 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -561,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K58"/>
+  <dimension ref="A2:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -839,6 +963,292 @@
       <c r="K57" s="2"/>
     </row>
     <row r="58" spans="1:11" ht="16" thickTop="1"/>
+    <row r="59" spans="1:11">
+      <c r="A59" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="3"/>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="3"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C63" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="3"/>
+      <c r="C64" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="3"/>
+      <c r="C65" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" s="3"/>
+      <c r="C66" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" s="3"/>
+      <c r="C67" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" s="3"/>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C69" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="3"/>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C71" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" s="3"/>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="16" thickBot="1">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+    </row>
+    <row r="75" spans="1:11" ht="16" thickTop="1"/>
+    <row r="76" spans="1:11">
+      <c r="A76" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77" s="3"/>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" s="4"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
+      <c r="A81" s="4"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
+      <c r="A82" s="4"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
+      <c r="A83" s="4"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
+      <c r="A84" s="4"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
+      <c r="A85" s="4"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
+      <c r="A86" s="3"/>
+    </row>
+    <row r="87" spans="1:11">
+      <c r="A87" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C87" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
+      <c r="A88" s="3"/>
+    </row>
+    <row r="89" spans="1:11">
+      <c r="A89" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C89" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
+      <c r="A90" s="3"/>
+    </row>
+    <row r="91" spans="1:11">
+      <c r="A91" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="16" thickBot="1">
+      <c r="A92" s="2"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
+    </row>
+    <row r="93" spans="1:11" ht="16" thickTop="1"/>
+    <row r="94" spans="1:11">
+      <c r="A94" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C94" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
+      <c r="A95" s="3"/>
+    </row>
+    <row r="96" spans="1:11">
+      <c r="A96" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C96" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="3"/>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C98" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="3"/>
+      <c r="C99" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="3"/>
+      <c r="C100" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="3"/>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C102" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="3"/>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C104" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="3"/>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>